<commit_message>
tests updated on 30/08/2018
</commit_message>
<xml_diff>
--- a/Resources/Crm_TestData.xlsx
+++ b/Resources/Crm_TestData.xlsx
@@ -33,9 +33,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Mr</t>
-  </si>
-  <si>
     <t>Rajesh</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>rajesh_negi75@yahoo.com</t>
   </si>
   <si>
-    <t>Dr</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>tomharry@gmail.com</t>
   </si>
   <si>
-    <t>Mrs</t>
-  </si>
-  <si>
     <t>Sunny</t>
   </si>
   <si>
@@ -67,6 +58,15 @@
   </si>
   <si>
     <t>sunnyleone@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,53 +445,53 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>7263871558</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>9808908909</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>9898989898</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>